<commit_message>
Added more annotated images
</commit_message>
<xml_diff>
--- a/Testcounts/averagehumancounts.xlsx
+++ b/Testcounts/averagehumancounts.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ed/Documents/GitHub/Buchnearer/Testcounts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57F1B5FC-BFFA-644F-9AA2-8F389E291D2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF644EAF-F50C-AC44-98AC-1A4E4FBEFE18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="460" windowWidth="18780" windowHeight="15820" xr2:uid="{A4CA6B42-0590-334B-B527-C0EA211502EC}"/>
+    <workbookView xWindow="12680" yWindow="460" windowWidth="16300" windowHeight="15820" xr2:uid="{A4CA6B42-0590-334B-B527-C0EA211502EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -435,47 +435,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D853E80-1E53-8A49-9397-EF9AD7AEDAA8}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="B1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="78.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="78.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
         <v>0</v>
-      </c>
-      <c r="B2">
-        <v>195</v>
       </c>
       <c r="C2">
         <v>195</v>
@@ -487,16 +484,23 @@
         <v>195</v>
       </c>
       <c r="F2">
-        <f>AVERAGE(B2,C2,D2,E2)</f>
         <v>195</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="G2">
+        <f t="shared" ref="G2:G11" si="0">AVERAGE(C2,D2,E2,F2)</f>
+        <v>195</v>
+      </c>
+      <c r="H2">
+        <v>146</v>
+      </c>
+      <c r="I2">
+        <f>H2/G2</f>
+        <v>0.74871794871794872</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>1</v>
-      </c>
-      <c r="B3">
-        <v>212</v>
       </c>
       <c r="C3">
         <v>212</v>
@@ -508,16 +512,23 @@
         <v>212</v>
       </c>
       <c r="F3">
-        <f>AVERAGE(B3,C3,D3,E3)</f>
         <v>212</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>212</v>
+      </c>
+      <c r="H3">
+        <v>170</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I11" si="1">H3/G3</f>
+        <v>0.80188679245283023</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
         <v>2</v>
-      </c>
-      <c r="B4">
-        <v>185</v>
       </c>
       <c r="C4">
         <v>185</v>
@@ -529,16 +540,23 @@
         <v>185</v>
       </c>
       <c r="F4">
-        <f>AVERAGE(B4,C4,D4,E4)</f>
         <v>185</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>185</v>
+      </c>
+      <c r="H4">
+        <v>162</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>0.87567567567567572</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
         <v>3</v>
-      </c>
-      <c r="B5">
-        <v>143</v>
       </c>
       <c r="C5">
         <v>143</v>
@@ -550,16 +568,23 @@
         <v>143</v>
       </c>
       <c r="F5">
-        <f>AVERAGE(B5,C5,D5,E5)</f>
         <v>143</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>143</v>
+      </c>
+      <c r="H5">
+        <v>126</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>0.88111888111888115</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
         <v>4</v>
-      </c>
-      <c r="B6">
-        <v>87</v>
       </c>
       <c r="C6">
         <v>87</v>
@@ -571,16 +596,23 @@
         <v>87</v>
       </c>
       <c r="F6">
-        <f>AVERAGE(B6,C6,D6,E6)</f>
         <v>87</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>87</v>
+      </c>
+      <c r="H6">
+        <v>79</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>0.90804597701149425</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
         <v>5</v>
-      </c>
-      <c r="B7">
-        <v>88</v>
       </c>
       <c r="C7">
         <v>88</v>
@@ -592,16 +624,23 @@
         <v>88</v>
       </c>
       <c r="F7">
-        <f>AVERAGE(B7,C7,D7,E7)</f>
         <v>88</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="H7">
+        <v>88</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
         <v>6</v>
-      </c>
-      <c r="B8">
-        <v>130</v>
       </c>
       <c r="C8">
         <v>130</v>
@@ -613,16 +652,23 @@
         <v>130</v>
       </c>
       <c r="F8">
-        <f>AVERAGE(B8,C8,D8,E8)</f>
         <v>130</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="H8">
+        <v>126</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>0.96923076923076923</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
         <v>12</v>
-      </c>
-      <c r="B9">
-        <v>139</v>
       </c>
       <c r="C9">
         <v>139</v>
@@ -634,16 +680,23 @@
         <v>139</v>
       </c>
       <c r="F9">
-        <f>AVERAGE(B9,C9,D9,E9)</f>
         <v>139</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>139</v>
+      </c>
+      <c r="H9">
+        <v>152</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>1.0935251798561152</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
         <v>13</v>
-      </c>
-      <c r="B10">
-        <v>65</v>
       </c>
       <c r="C10">
         <v>65</v>
@@ -655,16 +708,23 @@
         <v>65</v>
       </c>
       <c r="F10">
-        <f>AVERAGE(B10,C10,D10,E10)</f>
         <v>65</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="H10">
+        <v>61</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>0.93846153846153846</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
         <v>14</v>
-      </c>
-      <c r="B11">
-        <v>274</v>
       </c>
       <c r="C11">
         <v>274</v>
@@ -676,8 +736,24 @@
         <v>274</v>
       </c>
       <c r="F11">
-        <f>AVERAGE(B11,C11,D11,E11)</f>
         <v>274</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>274</v>
+      </c>
+      <c r="H11">
+        <v>227</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>0.82846715328467158</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I12">
+        <f>AVERAGE(I2:I11)</f>
+        <v>0.90451299158099252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>